<commit_message>
make events driver compatible with measures
</commit_message>
<xml_diff>
--- a/Tools/LIFEnet/NXr_866_measure_scenario_1.xlsx
+++ b/Tools/LIFEnet/NXr_866_measure_scenario_1.xlsx
@@ -4,16 +4,44 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="17280" windowHeight="9825"/>
+    <workbookView xWindow="180" yWindow="150" windowWidth="18315" windowHeight="9825"/>
   </bookViews>
   <sheets>
     <sheet name="NXr_866-meas1" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="eventOutput_1" localSheetId="0">'NXr_866-meas1'!$A$3:$J$45</definedName>
+    <definedName name="eventOutput_1" localSheetId="0">'NXr_866-meas1'!$A$3:$L$45</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>brownd9684</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Commonly indexed points are: 
+Battery Cabinets on UPS systems.
+Temp semsors of Cooling systems.
+Where: 0 is the first, 1 is the second,
+etc.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="110">
   <si>
     <t>PointId</t>
   </si>
@@ -351,9 +379,6 @@
     <t xml:space="preserve">IP= </t>
   </si>
   <si>
-    <t>126.4.100.101</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -374,13 +399,19 @@
   <si>
     <t>Run
 y / n</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>multi-module index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +573,12 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1002,7 +1039,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1028,10 +1065,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1068,6 +1101,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1410,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1425,41 +1461,44 @@
     <col min="5" max="5" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="22"/>
+    <col min="12" max="12" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="24"/>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="47.25">
+      <c r="H1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="47.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1472,29 +1511,32 @@
       <c r="D2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>98</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>4097</v>
       </c>
@@ -1516,20 +1558,23 @@
       <c r="G3">
         <v>3000</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="25">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>4099</v>
       </c>
@@ -1551,20 +1596,23 @@
       <c r="G4">
         <v>4000</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="H4" s="25">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4101</v>
       </c>
@@ -1586,20 +1634,23 @@
       <c r="G5">
         <v>5000</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="11">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="25">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>4113</v>
       </c>
@@ -1621,20 +1672,23 @@
       <c r="G6">
         <v>100</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="15">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="H6" s="25">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>4114</v>
       </c>
@@ -1656,20 +1710,23 @@
       <c r="G7">
         <v>200</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="25">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>4115</v>
       </c>
@@ -1691,20 +1748,23 @@
       <c r="G8">
         <v>300</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="H8" s="25">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>4105</v>
       </c>
@@ -1726,20 +1786,23 @@
       <c r="G9">
         <v>599</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="H9" s="25">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>4096</v>
       </c>
@@ -1761,20 +1824,23 @@
       <c r="G10">
         <v>2500</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="H10" s="25">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>4098</v>
       </c>
@@ -1796,20 +1862,23 @@
       <c r="G11">
         <v>3500</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="H11" s="25">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>4100</v>
       </c>
@@ -1831,20 +1900,23 @@
       <c r="G12">
         <v>4500</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="H12" s="25">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>4116</v>
       </c>
@@ -1866,17 +1938,20 @@
       <c r="G13">
         <v>7000</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-      <c r="K13" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="H13" s="25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>4117</v>
       </c>
@@ -1898,17 +1973,20 @@
       <c r="G14">
         <v>8000</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0</v>
-      </c>
-      <c r="K14" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="H14" s="25">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>4118</v>
       </c>
@@ -1930,17 +2008,20 @@
       <c r="G15">
         <v>9000</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="H15" s="25">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>4128</v>
       </c>
@@ -1962,20 +2043,23 @@
       <c r="G16">
         <v>1500</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="H16" s="25">
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>4129</v>
       </c>
@@ -1997,20 +2081,23 @@
       <c r="G17">
         <v>1750</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17" s="15">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="H17" s="25">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>4130</v>
       </c>
@@ -2032,20 +2119,23 @@
       <c r="G18">
         <v>2000</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="15">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="H18" s="25">
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>4131</v>
       </c>
@@ -2067,20 +2157,23 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="H19" s="25">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>4150</v>
       </c>
@@ -2102,20 +2195,23 @@
       <c r="G20">
         <v>1000000</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="H20" s="25">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>4155</v>
       </c>
@@ -2137,20 +2233,23 @@
       <c r="G21">
         <v>480</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="H21" s="25">
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>4156</v>
       </c>
@@ -2172,20 +2271,23 @@
       <c r="G22">
         <v>100</v>
       </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="15">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="H22" s="25">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>4291</v>
       </c>
@@ -2207,20 +2309,23 @@
       <c r="G23">
         <v>200</v>
       </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="H23" s="25">
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>4149</v>
       </c>
@@ -2242,20 +2347,23 @@
       <c r="G24">
         <v>1000</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" s="15">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="H24" s="25">
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>4385</v>
       </c>
@@ -2277,20 +2385,23 @@
       <c r="G25">
         <v>5500</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25" s="15">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K25" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>4386</v>
       </c>
@@ -2312,20 +2423,23 @@
       <c r="G26">
         <v>6500</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26" s="15">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="H26" s="25">
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K26" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>4387</v>
       </c>
@@ -2347,20 +2461,23 @@
       <c r="G27">
         <v>7500</v>
       </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27" s="15">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="H27" s="25">
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>4204</v>
       </c>
@@ -2382,20 +2499,23 @@
       <c r="G28">
         <v>20</v>
       </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28" s="15">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="H28" s="25">
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K28" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>4205</v>
       </c>
@@ -2417,20 +2537,23 @@
       <c r="G29">
         <v>30</v>
       </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29" s="15">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="H29" s="25">
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K29" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>4206</v>
       </c>
@@ -2452,20 +2575,23 @@
       <c r="G30">
         <v>40</v>
       </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="I30" s="15">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="H30" s="25">
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>4207</v>
       </c>
@@ -2487,20 +2613,23 @@
       <c r="G31">
         <v>799</v>
       </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31" s="15">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="H31" s="25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K31" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>4201</v>
       </c>
@@ -2522,20 +2651,23 @@
       <c r="G32">
         <v>1000</v>
       </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32" s="15">
-        <v>0</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="H32" s="25">
+        <v>0</v>
+      </c>
+      <c r="I32" s="13">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>4202</v>
       </c>
@@ -2557,20 +2689,23 @@
       <c r="G33">
         <v>2000</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33" s="15">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="H33" s="25">
+        <v>0</v>
+      </c>
+      <c r="I33" s="13">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>4203</v>
       </c>
@@ -2592,20 +2727,23 @@
       <c r="G34">
         <v>3000</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34" s="15">
-        <v>0</v>
-      </c>
-      <c r="J34" s="1" t="s">
+      <c r="H34" s="25">
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K34" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>4210</v>
       </c>
@@ -2627,17 +2765,20 @@
       <c r="G35">
         <v>5000</v>
       </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35" s="15">
-        <v>0</v>
-      </c>
-      <c r="K35" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="H35" s="25">
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>4211</v>
       </c>
@@ -2659,17 +2800,20 @@
       <c r="G36">
         <v>6000</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="15">
-        <v>0</v>
-      </c>
-      <c r="K36" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="H36" s="25">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>4212</v>
       </c>
@@ -2691,17 +2835,20 @@
       <c r="G37">
         <v>7000</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37" s="15">
-        <v>0</v>
-      </c>
-      <c r="K37" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="H37" s="25">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>4223</v>
       </c>
@@ -2723,20 +2870,23 @@
       <c r="G38">
         <v>100000</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38" s="15">
-        <v>0</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="H38" s="25">
+        <v>0</v>
+      </c>
+      <c r="I38" s="13">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>4224</v>
       </c>
@@ -2758,20 +2908,23 @@
       <c r="G39">
         <v>200000</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39" s="15">
-        <v>0</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="H39" s="25">
+        <v>0</v>
+      </c>
+      <c r="I39" s="13">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>4225</v>
       </c>
@@ -2793,20 +2946,23 @@
       <c r="G40">
         <v>300000</v>
       </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40" s="15">
-        <v>0</v>
-      </c>
-      <c r="J40" s="1" t="s">
+      <c r="H40" s="25">
+        <v>0</v>
+      </c>
+      <c r="I40" s="13">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L40" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>4209</v>
       </c>
@@ -2828,20 +2984,23 @@
       <c r="G41">
         <v>400000</v>
       </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41" s="15">
-        <v>0</v>
-      </c>
-      <c r="J41" s="1" t="s">
+      <c r="H41" s="25">
+        <v>0</v>
+      </c>
+      <c r="I41" s="13">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K41" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>4208</v>
       </c>
@@ -2863,20 +3022,23 @@
       <c r="G42">
         <v>500000</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="I42" s="15">
-        <v>0</v>
-      </c>
-      <c r="J42" s="1" t="s">
+      <c r="H42" s="25">
+        <v>0</v>
+      </c>
+      <c r="I42" s="13">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>5159</v>
       </c>
@@ -2898,17 +3060,20 @@
       <c r="G43">
         <v>10</v>
       </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43" s="15">
-        <v>0</v>
-      </c>
-      <c r="K43" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="H43" s="25">
+        <v>0</v>
+      </c>
+      <c r="I43" s="13">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>5160</v>
       </c>
@@ -2930,17 +3095,20 @@
       <c r="G44">
         <v>20</v>
       </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="I44" s="15">
-        <v>0</v>
-      </c>
-      <c r="K44" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="H44" s="25">
+        <v>0</v>
+      </c>
+      <c r="I44" s="13">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>5161</v>
       </c>
@@ -2962,14 +3130,452 @@
       <c r="G45">
         <v>30</v>
       </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45" s="15">
-        <v>0</v>
-      </c>
-      <c r="K45" s="26" t="s">
-        <v>107</v>
+      <c r="H45" s="25">
+        <v>0</v>
+      </c>
+      <c r="I45" s="13">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="H46" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="H47" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="H48" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8">
+      <c r="H49" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8">
+      <c r="H50" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8">
+      <c r="H51" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8">
+      <c r="H52" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8">
+      <c r="H53" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8">
+      <c r="H54" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8">
+      <c r="H55" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8">
+      <c r="H56" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8">
+      <c r="H57" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8">
+      <c r="H58" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8">
+      <c r="H59" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8">
+      <c r="H60" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8">
+      <c r="H61" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8">
+      <c r="H62" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8">
+      <c r="H63" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8">
+      <c r="H64" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8">
+      <c r="H65" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8">
+      <c r="H66" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8">
+      <c r="H67" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8">
+      <c r="H68" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8">
+      <c r="H69" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8">
+      <c r="H70" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8">
+      <c r="H71" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8">
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8">
+      <c r="H73" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8">
+      <c r="H74" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8">
+      <c r="H75" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8">
+      <c r="H76" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8">
+      <c r="H77" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8">
+      <c r="H78" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8">
+      <c r="H79" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="8:8">
+      <c r="H80" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8">
+      <c r="H81" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8">
+      <c r="H82" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8">
+      <c r="H83" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8">
+      <c r="H84" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8">
+      <c r="H85" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8">
+      <c r="H86" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8">
+      <c r="H87" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8">
+      <c r="H88" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8">
+      <c r="H89" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8">
+      <c r="H90" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8">
+      <c r="H91" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8">
+      <c r="H92" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8">
+      <c r="H93" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8">
+      <c r="H94" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8">
+      <c r="H95" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8">
+      <c r="H96" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="8:8">
+      <c r="H97" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="8:8">
+      <c r="H98" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8">
+      <c r="H99" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8">
+      <c r="H100" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8">
+      <c r="H101" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8">
+      <c r="H102" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8">
+      <c r="H103" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8">
+      <c r="H104" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8">
+      <c r="H105" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8">
+      <c r="H106" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="8:8">
+      <c r="H107" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="8:8">
+      <c r="H108" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8">
+      <c r="H109" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="8:8">
+      <c r="H110" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="8:8">
+      <c r="H111" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="8:8">
+      <c r="H112" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="8:8">
+      <c r="H113" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="8:8">
+      <c r="H114" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="8:8">
+      <c r="H115" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8">
+      <c r="H116" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="8:8">
+      <c r="H117" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8">
+      <c r="H118" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="8:8">
+      <c r="H119" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="8:8">
+      <c r="H120" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="8:8">
+      <c r="H121" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="8:8">
+      <c r="H122" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="8:8">
+      <c r="H123" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="8:8">
+      <c r="H124" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="8:8">
+      <c r="H125" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="8:8">
+      <c r="H126" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="8:8">
+      <c r="H127" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="8:8">
+      <c r="H128" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="8:8">
+      <c r="H129" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="8:8">
+      <c r="H130" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="8:8">
+      <c r="H131" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="8:8">
+      <c r="H132" s="25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2978,5 +3584,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>